<commit_message>
Add new combat tactics, balancing of existing, new combat phase
</commit_message>
<xml_diff>
--- a/Modding resources/Land combat/tactics.xlsx
+++ b/Modding resources/Land combat/tactics.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yauheni_Papiunenka\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gene\Documents\Paradox Interactive\Hearts of Iron IV\mod\md\Modding resources\Land combat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669C6AA9-F80C-4F45-9C62-AC94CEDB293A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{43BB485A-628B-4F39-A204-1E9C8DA3291E}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="77">
   <si>
     <t>common</t>
   </si>
@@ -224,12 +224,54 @@
   </si>
   <si>
     <t>6c</t>
+  </si>
+  <si>
+    <t>Limited recon</t>
+  </si>
+  <si>
+    <t>Aggressive recon</t>
+  </si>
+  <si>
+    <t>Recon Attack</t>
+  </si>
+  <si>
+    <t>Supression advance</t>
+  </si>
+  <si>
+    <t>Mobile recon</t>
+  </si>
+  <si>
+    <t>breakthrough recon</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>Defense</t>
+  </si>
+  <si>
+    <t>Recon defense</t>
+  </si>
+  <si>
+    <t>Hunter packs</t>
+  </si>
+  <si>
+    <t>Ambush formation</t>
+  </si>
+  <si>
+    <t>Counter battery</t>
+  </si>
+  <si>
+    <t>Node defense</t>
+  </si>
+  <si>
+    <t>Pincer manouver</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -584,29 +626,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873C94C9-E574-4252-A504-CFECAD7EDB64}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="25.77734375" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" customWidth="1"/>
-    <col min="9" max="9" width="24.33203125" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
@@ -626,7 +668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -640,7 +682,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>3</v>
       </c>
@@ -651,7 +693,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>4</v>
       </c>
@@ -665,7 +707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>5</v>
       </c>
@@ -676,7 +718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>6</v>
       </c>
@@ -690,12 +732,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>20</v>
       </c>
@@ -712,7 +754,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>22</v>
       </c>
@@ -729,7 +771,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>24</v>
       </c>
@@ -746,7 +788,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>26</v>
       </c>
@@ -763,7 +805,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>28</v>
       </c>
@@ -771,7 +813,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>35</v>
       </c>
@@ -779,7 +821,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>37</v>
       </c>
@@ -787,7 +829,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>39</v>
       </c>
@@ -795,7 +837,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>41</v>
       </c>
@@ -803,7 +845,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>32</v>
       </c>
@@ -811,7 +853,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>22</v>
       </c>
@@ -828,7 +870,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>32</v>
       </c>
@@ -851,7 +893,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
         <v>27</v>
       </c>
@@ -862,7 +904,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
         <v>49</v>
       </c>
@@ -873,7 +915,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>39</v>
       </c>
@@ -890,7 +932,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>24</v>
       </c>
@@ -898,7 +940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>37</v>
       </c>
@@ -921,7 +963,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>41</v>
       </c>
@@ -944,12 +986,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L30" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>22</v>
       </c>
@@ -957,7 +999,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>26</v>
       </c>
@@ -965,7 +1007,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>32</v>
       </c>
@@ -977,4 +1019,81 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E11:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="11" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>